<commit_message>
Edited cell calculations for Balance and Total Sell Price. Added 'push main table to backup' button & functionality. Added basic filters on Dashboard page.
</commit_message>
<xml_diff>
--- a/data/inventory.xlsx
+++ b/data/inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,31 +495,31 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>1925</v>
+        <v>2200</v>
       </c>
       <c r="E2" t="n">
         <v>275</v>
       </c>
       <c r="F2" t="n">
-        <v>-2730</v>
+        <v>3120</v>
       </c>
       <c r="G2" t="n">
-        <v>3120</v>
+        <v>390</v>
       </c>
       <c r="H2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
-        <v>114</v>
+        <v>35</v>
       </c>
       <c r="K2" t="n">
-        <v>114</v>
+        <v>535</v>
       </c>
     </row>
     <row r="3">
@@ -532,19 +532,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" t="n">
-        <v>2656</v>
+        <v>1660</v>
       </c>
       <c r="E3" t="n">
         <v>332</v>
       </c>
       <c r="F3" t="n">
-        <v>8000</v>
+        <v>2500</v>
       </c>
       <c r="G3" t="n">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
@@ -561,54 +561,25 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>1210</v>
+        <v>405</v>
       </c>
       <c r="E4" t="n">
-        <v>605</v>
+        <v>405</v>
       </c>
       <c r="F4" t="n">
-        <v>-5975</v>
+        <v>625</v>
       </c>
       <c r="G4" t="n">
-        <v>3300</v>
+        <v>625</v>
       </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Lamp</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>375</v>
-      </c>
-      <c r="E5" t="n">
-        <v>125</v>
-      </c>
-      <c r="F5" t="n">
-        <v>741</v>
-      </c>
-      <c r="G5" t="n">
-        <v>247</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>